<commit_message>
added diary entry for Aman Bhatia
</commit_message>
<xml_diff>
--- a/diaries/diary-AmanBhatia.xlsx
+++ b/diaries/diary-AmanBhatia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanbhatia/Documents/Coursework/Quarter2/Reverse Engineering/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3753B8A2-D5DF-A04D-8953-C01E94C9A58C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A64546C-567B-6842-9F08-E513CCCFCD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Achievements</t>
   </si>
   <si>
-    <t>Etc.</t>
-  </si>
-  <si>
     <t>Aman Bhatia</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>10pm - 10:30 pm</t>
   </si>
   <si>
-    <t>Anjana, Vaishakhi</t>
-  </si>
-  <si>
     <t>Team formation</t>
   </si>
   <si>
@@ -130,6 +124,48 @@
   </si>
   <si>
     <t>felt challenged while working on this task</t>
+  </si>
+  <si>
+    <t>To understand the technicalities of Reverse Engineering, by actually analyzing code, and try to find the causes of bugs.</t>
+  </si>
+  <si>
+    <t>Reverse engineering is not easy, but a little understanding can help us in finding beacons, which can guide us to the correct answer, in todays lecture, this correct answer was the location of the bugs/feature</t>
+  </si>
+  <si>
+    <t>We were able to find more or less the precise causes of bugs, in JPacMan 1 and 2, by finding usages of relevant classes,methods,keywords.Used various approaches like opportunist,bottom up etc.</t>
+  </si>
+  <si>
+    <t>excited</t>
+  </si>
+  <si>
+    <t>6:00 - 10:00pm</t>
+  </si>
+  <si>
+    <t>Anjana, Vaishakhi,Myself</t>
+  </si>
+  <si>
+    <t>To decide on a group projct</t>
+  </si>
+  <si>
+    <t>After reading a lot of projects, we finally found a relevant one -OpenRefine</t>
+  </si>
+  <si>
+    <t>It is very difficult to find the "perfect" project, some of them have cryptic looking code, but a rich documentation, while others lack a documentation</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>10:00 am - 12:30 pm</t>
+  </si>
+  <si>
+    <t>To finsih the homework, and understand how we could add new features to an existing codebase</t>
+  </si>
+  <si>
+    <t>Was able to understand what the homework asked of me. Explored JPacMan3, and understood, the process of building up on already existing code.</t>
+  </si>
+  <si>
+    <t>If the code employs good coding practices, like proper nomenclature of variables, proper method names, comments, it. Becomes slightly easier to understand code, even if somebody else had written it. The third question was interesting, since I felt, it could be done in more than one way</t>
   </si>
 </sst>
 </file>
@@ -294,14 +330,14 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -623,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,24 +669,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -666,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -678,8 +714,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>13</v>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -691,8 +727,8 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>14</v>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -742,102 +778,142 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>43839</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="8" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>43843</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>43843</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="G11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>43844</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>43844</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="7" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>43846</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="E13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>43848</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>43850</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>

</xml_diff>

<commit_message>
Added diary entry for Aman Bhatia 30tj January
</commit_message>
<xml_diff>
--- a/diaries/diary-AmanBhatia.xlsx
+++ b/diaries/diary-AmanBhatia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanbhatia/Documents/Coursework/Quarter2/Reverse Engineering/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A64546C-567B-6842-9F08-E513CCCFCD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7A70A1-CB20-AA48-86E8-DD9A1702AE69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -166,6 +166,90 @@
   </si>
   <si>
     <t>If the code employs good coding practices, like proper nomenclature of variables, proper method names, comments, it. Becomes slightly easier to understand code, even if somebody else had written it. The third question was interesting, since I felt, it could be done in more than one way</t>
+  </si>
+  <si>
+    <t>Was unwell,could'nt attend the class</t>
+  </si>
+  <si>
+    <t>Asked my friend, to take notes, so I could learn what I missed in the lecture.</t>
+  </si>
+  <si>
+    <t>Asked about what I had missed, so I could   do my own work, before my friend explained the class work to me</t>
+  </si>
+  <si>
+    <t>Was able to get a brief idea, about mental maps, and uml diagrams</t>
+  </si>
+  <si>
+    <t>Not that good, since I was unwell</t>
+  </si>
+  <si>
+    <t>12:00 - 3:00 pm</t>
+  </si>
+  <si>
+    <t>Vaishakhi,Anjana</t>
+  </si>
+  <si>
+    <t>Selecting a new project</t>
+  </si>
+  <si>
+    <t>Selected h2 database, since it reflected our interests better than openRefine, we then build the project, made it work, and submitted a pull request</t>
+  </si>
+  <si>
+    <t>It was difficult understanding the project that most interests us, since there are a myriad of interesting projects out there, h2 however seemed to grab our attention</t>
+  </si>
+  <si>
+    <t>elated, since our pull request was approved.</t>
+  </si>
+  <si>
+    <t>8:00-10:00pm</t>
+  </si>
+  <si>
+    <t>Start working on the homework and UML diagrams, learn what I had missed in class in detail</t>
+  </si>
+  <si>
+    <t>We created the UML diagram and decided to work on two features - 1.Create Table
+2.Set User Priveleges(admin/not admin)
+Learn about Mental Mapping/UML diagrams(was already comfortable with UML diagrams, so was able to grasp it all)
+Also learnt about the JPACMAN activity that I had missed in the class. Understood how we can use the templates to accelerate and organize our search for features</t>
+  </si>
+  <si>
+    <t>The UML diagrams for h2 database are complex, without organization, it can become tricky to zero in on a particular feature</t>
+  </si>
+  <si>
+    <t>confused, about the approach, but positive that we will do it.</t>
+  </si>
+  <si>
+    <t>10:00pm - 1:00am</t>
+  </si>
+  <si>
+    <t>Vaihakhi,Anjana</t>
+  </si>
+  <si>
+    <t>Continued working on the homework</t>
+  </si>
+  <si>
+    <t>It took some time to understand where the features are implemented.We understood,where the features were, and how its being called from various places in the code</t>
+  </si>
+  <si>
+    <t>We used the find usages feature in intellij to zero in on files we thought are relevant, and kept track of them according to the template.</t>
+  </si>
+  <si>
+    <t>neutral, we know we found relevant classes, and methods, but feel that we might be missing a piece, we will keep on working on it though.</t>
+  </si>
+  <si>
+    <t>10:00 am - 1:00 pm</t>
+  </si>
+  <si>
+    <t>Prepare the report</t>
+  </si>
+  <si>
+    <t>Prepared a report that explains our search by making use of the templates</t>
+  </si>
+  <si>
+    <t>It becomes easy to search, and find features if we have an organized approach(templates)</t>
+  </si>
+  <si>
+    <t>happy, that we finally finsihed it.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +388,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -338,6 +422,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -659,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="156" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -915,50 +1006,120 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>43853</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>43856</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>43856</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>43859</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>

</xml_diff>

<commit_message>
Aman Bhatia diary updated 6th February 20
</commit_message>
<xml_diff>
--- a/diaries/diary-AmanBhatia.xlsx
+++ b/diaries/diary-AmanBhatia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanbhatia/Documents/Coursework/Quarter2/Reverse Engineering/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7A70A1-CB20-AA48-86E8-DD9A1702AE69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5A601E-DC10-4A44-B786-0D9CF6789F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -250,6 +250,81 @@
   </si>
   <si>
     <t>happy, that we finally finsihed it.</t>
+  </si>
+  <si>
+    <t>Learn about key practices in Reverse Engineering and various ways to model the architecture</t>
+  </si>
+  <si>
+    <t>Understood how important it is to go as deep as we can into the code, to fully understand a feature. Improper understanding can lead to wrong assumptions, and in the future these assumptions might cost us.</t>
+  </si>
+  <si>
+    <t>Excited to learn some new ways to model the flow, call graphs, sequence diagrams. Understood, the importance of going in depth, and revisiting the code, to solidify our understanding</t>
+  </si>
+  <si>
+    <t>excited to learn new ways to model the code and flow.</t>
+  </si>
+  <si>
+    <t>Deciding on the features 1. how does the h2 database support embedded and server mode
+2. How is data actually persisted from h2 onto our disk.</t>
+  </si>
+  <si>
+    <t>We were able to figure out our first feature. For the second, we started with our work, and decided to continue working on it on the next day.</t>
+  </si>
+  <si>
+    <t>Before we got into working on our feature, we were facing some issues with running our application. Tools.jar file was not being detected in pom.xml. So we had to downgrade our java version, edit the system path in pom.xml to reflect the location of tools.jar and do a maven clean.
+We figured, that things become really simpler, once the code uses proper naming conventions, and the names are reflective of their purpose. Find usages, is a great way to explore the codebase.</t>
+  </si>
+  <si>
+    <t>Neutral, at first, happy once we had figured the feature.</t>
+  </si>
+  <si>
+    <t>10:00pm - 12:00pm</t>
+  </si>
+  <si>
+    <t>Start working on the second feature</t>
+  </si>
+  <si>
+    <t>We were not able to fully deep dive into our second feature, and after spending the whole time, we decided to choose a different feature as our second option.
+Our new choice was "How does H2 database handle multiple commands like Insert/Deltete etc"</t>
+  </si>
+  <si>
+    <t>Sometimes it becomes really hard to understand a particular flow, we tried our best but couldn't fully understand it, so we concluded that we would move on with a different choice</t>
+  </si>
+  <si>
+    <t>Sad, since we wanted to understand this, but we couldn't</t>
+  </si>
+  <si>
+    <t>10:pm - 2:00 am</t>
+  </si>
+  <si>
+    <t>Finish the work on new feature</t>
+  </si>
+  <si>
+    <t>This time we were able to understand the new feature that we had chosen, and were able to draw our diagrams.</t>
+  </si>
+  <si>
+    <t>It was very difficult working on the features especially with the second one, because we had to make a change with it.</t>
+  </si>
+  <si>
+    <t>Unhappy at first, but relaxed, since the new choice was understood by us.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00 am - 12:30 pm </t>
+  </si>
+  <si>
+    <t>Finish the report</t>
+  </si>
+  <si>
+    <t>We finished writing our report with all the diagrams.</t>
+  </si>
+  <si>
+    <t>Once we have everything understood, and written, writing a report bcomes easy</t>
+  </si>
+  <si>
+    <t>Excited, to learn about todays lecture.</t>
+  </si>
+  <si>
+    <t>11:00 am - 1:00pm and 9:30 pm - 11:00 pm</t>
   </si>
 </sst>
 </file>
@@ -420,15 +495,15 @@
     <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -750,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="156" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -760,24 +835,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1029,14 +1104,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
         <v>43856</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1052,7 +1127,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="221" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>43856</v>
       </c>
@@ -1062,7 +1137,7 @@
       <c r="C18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -1121,50 +1196,120 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
+    <row r="21" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>43867</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>

</xml_diff>

<commit_message>
Diary entry updated for Aman Bhatia
</commit_message>
<xml_diff>
--- a/diaries/diary-AmanBhatia.xlsx
+++ b/diaries/diary-AmanBhatia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanbhatia/Documents/Coursework/Quarter2/Reverse Engineering/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5A601E-DC10-4A44-B786-0D9CF6789F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD81193B-9132-FE41-A1FC-5BB33B725872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -325,6 +325,48 @@
   </si>
   <si>
     <t>11:00 am - 1:00pm and 9:30 pm - 11:00 pm</t>
+  </si>
+  <si>
+    <t>Learn about KEP4,5,6. Learn about mental simulations</t>
+  </si>
+  <si>
+    <t>Understood how experts approach reading and analyzing code. Reflecting back is one of the most important things to do.</t>
+  </si>
+  <si>
+    <t>Reflecting back, applying key expert practices will come slowly with time. Templates can help us achieve that slowly and steadily</t>
+  </si>
+  <si>
+    <t>Excited to listen to the guest lecture, and learn about these key practices.</t>
+  </si>
+  <si>
+    <t>9:00 pm - 10:00pm</t>
+  </si>
+  <si>
+    <t>Study a little bit for the mid term</t>
+  </si>
+  <si>
+    <t>Covered slides 1-3</t>
+  </si>
+  <si>
+    <t>The concepts are easy to read, but I understand their application will come over time</t>
+  </si>
+  <si>
+    <t>9:00pm - 11:00pm</t>
+  </si>
+  <si>
+    <t>Study more for the mid term</t>
+  </si>
+  <si>
+    <t>Covered slides 4 and 5 and UML notations</t>
+  </si>
+  <si>
+    <t>2/11/2020 and 2/12/2020</t>
+  </si>
+  <si>
+    <t>Concepts in the latter slides are a little less easy to grasp, but a revision would reinforce these</t>
+  </si>
+  <si>
+    <t>Neutral, a little tensed</t>
   </si>
 </sst>
 </file>
@@ -825,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="156" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="156" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1311,32 +1353,74 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
+    <row r="26" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>43867</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>43871</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>

</xml_diff>

<commit_message>
Diary entry updated for AmanBhatia
</commit_message>
<xml_diff>
--- a/diaries/diary-AmanBhatia.xlsx
+++ b/diaries/diary-AmanBhatia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanbhatia/Documents/Coursework/Quarter2/Reverse Engineering/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD81193B-9132-FE41-A1FC-5BB33B725872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71E583A-5830-4842-AD2A-4CCC8A58952F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="123">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -367,6 +367,45 @@
   </si>
   <si>
     <t>Neutral, a little tensed</t>
+  </si>
+  <si>
+    <t>Take the midterm, and learn about stakeholders</t>
+  </si>
+  <si>
+    <t>Learnt about various stakeholders of the system</t>
+  </si>
+  <si>
+    <t>Stakeholders of a system are not just limited to people who can affect or be affected by the system, stakeholders may also include organizations and people like donors, maintainers, users etc</t>
+  </si>
+  <si>
+    <t>Relaxed after the midterm</t>
+  </si>
+  <si>
+    <t>11:00 am - 2:00 pm</t>
+  </si>
+  <si>
+    <t>Resubmit homework 1</t>
+  </si>
+  <si>
+    <t>Resubmitted homework 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrary to our belief that our packet was strong, we realized the importance of "making it easy for a third person to read" our code. Slowly but surely we are understanding the need of proper and structured documentation, comments, diagrams that explain our approach. </t>
+  </si>
+  <si>
+    <t>11:00 pm - 12:30 am</t>
+  </si>
+  <si>
+    <t>Work on high level perspective(the big picture)</t>
+  </si>
+  <si>
+    <t>Identified stakeholders, system domain, and functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up untill now we have dived into the code. This assignment let us see our system from a broader perspective, By identifying the different kinds of stakeholder, I believe we can understand for instance what kind of organizations would use this system(H2), or what will people benefit out of it. We knew the domain of H2. We talked and understand how h2 is unique from other database options out there. </t>
+  </si>
+  <si>
+    <t>Relaxed</t>
   </si>
 </sst>
 </file>
@@ -867,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="156" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1422,32 +1461,74 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
+    <row r="29" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>43874</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="10">
+        <v>43877</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A31" s="10">
+        <v>43880</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>

</xml_diff>